<commit_message>
resposive video in home page
</commit_message>
<xml_diff>
--- a/make_lrt_json/LAT-content_Mod1_2.xlsx
+++ b/make_lrt_json/LAT-content_Mod1_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiadhgrandt-nesher/Workbench/aaa/make_lrt_json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB15251A-72C6-3A4D-A1EA-C3B2816EF595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E9DE65-022D-474D-8DD1-BFD8B8C4A420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47700" yWindow="-8960" windowWidth="40460" windowHeight="20080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Content by Screen" sheetId="1" r:id="rId1"/>
@@ -999,13 +999,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1017,6 +1010,13 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1239,11 +1239,11 @@
   </sheetPr>
   <dimension ref="A1:BC1025"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E33" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="W30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J76" sqref="J76"/>
+      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1291,46 +1291,46 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="29" t="s">
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
-      <c r="V1" s="29" t="s">
+      <c r="V1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="28"/>
-      <c r="X1" s="27" t="s">
+      <c r="W1" s="33"/>
+      <c r="X1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="3"/>
@@ -4707,10 +4707,10 @@
         <v>37</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="E39" s="18" t="s">
         <v>113</v>
@@ -4719,14 +4719,10 @@
         <v>21</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="H39" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="I39" s="18" t="s">
-        <v>122</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
       <c r="J39" s="17"/>
       <c r="K39" s="17"/>
       <c r="L39" s="17"/>
@@ -4742,7 +4738,7 @@
       <c r="V39" s="17"/>
       <c r="W39" s="17"/>
       <c r="X39" s="15">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="Y39" s="18" t="s">
         <v>35</v>
@@ -4755,7 +4751,7 @@
       </c>
       <c r="AB39" s="17"/>
       <c r="AC39" s="15">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="AD39" s="18" t="s">
         <v>37</v>
@@ -4763,7 +4759,7 @@
       <c r="AE39" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AF39" s="33" t="s">
+      <c r="AF39" s="30" t="s">
         <v>39</v>
       </c>
       <c r="AG39" s="9"/>
@@ -4774,10 +4770,10 @@
       <c r="AJ39" s="9"/>
       <c r="AK39" s="9"/>
       <c r="AL39" s="9"/>
-      <c r="AM39" s="15" t="s">
+      <c r="AM39" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="AN39" s="18"/>
+      <c r="AN39" s="17"/>
       <c r="AO39" s="9"/>
       <c r="AP39" s="9"/>
       <c r="AQ39" s="9"/>
@@ -4802,10 +4798,10 @@
         <v>38</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>113</v>
@@ -4814,10 +4810,10 @@
         <v>21</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="I40" s="18"/>
       <c r="J40" s="17"/>
@@ -4835,10 +4831,10 @@
       <c r="V40" s="17"/>
       <c r="W40" s="17"/>
       <c r="X40" s="15">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Y40" s="18" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="Z40" s="15" t="s">
         <v>22</v>
@@ -4848,7 +4844,7 @@
       </c>
       <c r="AB40" s="17"/>
       <c r="AC40" s="15">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="AD40" s="18" t="s">
         <v>37</v>
@@ -4856,7 +4852,7 @@
       <c r="AE40" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AF40" s="33" t="s">
+      <c r="AF40" s="30" t="s">
         <v>39</v>
       </c>
       <c r="AG40" s="9"/>
@@ -4867,10 +4863,10 @@
       <c r="AJ40" s="9"/>
       <c r="AK40" s="9"/>
       <c r="AL40" s="9"/>
-      <c r="AM40" s="15" t="s">
+      <c r="AM40" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="AN40" s="18"/>
+      <c r="AN40" s="17"/>
       <c r="AO40" s="9"/>
       <c r="AP40" s="9"/>
       <c r="AQ40" s="9"/>
@@ -4895,10 +4891,10 @@
         <v>39</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="E41" s="18" t="s">
         <v>113</v>
@@ -4913,7 +4909,7 @@
         <v>128</v>
       </c>
       <c r="I41" s="17"/>
-      <c r="J41" s="34" t="s">
+      <c r="J41" s="31" t="s">
         <v>212</v>
       </c>
       <c r="K41" s="18" t="s">
@@ -4945,10 +4941,10 @@
         <v>38</v>
       </c>
       <c r="AB41" s="18" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AC41" s="15">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AD41" s="18" t="s">
         <v>132</v>
@@ -4997,10 +4993,10 @@
         <v>40</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="E42" s="18" t="s">
         <v>113</v>
@@ -5009,10 +5005,10 @@
         <v>21</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
+        <v>142</v>
+      </c>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
       <c r="J42" s="17"/>
       <c r="K42" s="17"/>
       <c r="L42" s="17"/>
@@ -5028,7 +5024,7 @@
       <c r="V42" s="17"/>
       <c r="W42" s="17"/>
       <c r="X42" s="15">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="Y42" s="18" t="s">
         <v>35</v>
@@ -5041,7 +5037,7 @@
       </c>
       <c r="AB42" s="17"/>
       <c r="AC42" s="15">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="AD42" s="18" t="s">
         <v>37</v>
@@ -5049,7 +5045,7 @@
       <c r="AE42" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AF42" s="33" t="s">
+      <c r="AF42" s="30" t="s">
         <v>39</v>
       </c>
       <c r="AG42" s="9"/>
@@ -5088,10 +5084,10 @@
         <v>41</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="E43" s="18" t="s">
         <v>113</v>
@@ -5100,12 +5096,14 @@
         <v>21</v>
       </c>
       <c r="G43" s="18" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="I43" s="18"/>
+        <v>144</v>
+      </c>
+      <c r="I43" s="18" t="s">
+        <v>145</v>
+      </c>
       <c r="J43" s="17"/>
       <c r="K43" s="17"/>
       <c r="L43" s="17"/>
@@ -5121,10 +5119,10 @@
       <c r="V43" s="17"/>
       <c r="W43" s="17"/>
       <c r="X43" s="15">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="Y43" s="18" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="Z43" s="15" t="s">
         <v>22</v>
@@ -5134,7 +5132,7 @@
       </c>
       <c r="AB43" s="17"/>
       <c r="AC43" s="15">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="AD43" s="18" t="s">
         <v>37</v>
@@ -5142,7 +5140,7 @@
       <c r="AE43" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AF43" s="33" t="s">
+      <c r="AF43" s="30" t="s">
         <v>39</v>
       </c>
       <c r="AG43" s="9"/>
@@ -5181,10 +5179,10 @@
         <v>42</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="E44" s="18" t="s">
         <v>113</v>
@@ -5199,7 +5197,7 @@
         <v>128</v>
       </c>
       <c r="I44" s="17"/>
-      <c r="J44" s="34" t="s">
+      <c r="J44" s="31" t="s">
         <v>212</v>
       </c>
       <c r="K44" s="18" t="s">
@@ -5231,10 +5229,10 @@
         <v>38</v>
       </c>
       <c r="AB44" s="18" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AC44" s="15">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AD44" s="18" t="s">
         <v>132</v>
@@ -5275,96 +5273,102 @@
       <c r="BB44" s="9"/>
       <c r="BC44" s="9"/>
     </row>
-    <row r="45" spans="1:55" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:55" s="29" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
         <v>111</v>
       </c>
       <c r="B45" s="20">
         <v>43</v>
       </c>
-      <c r="C45" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="E45" s="18" t="s">
+      <c r="C45" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="F45" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G45" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="17"/>
-      <c r="K45" s="17"/>
-      <c r="L45" s="17"/>
-      <c r="M45" s="17"/>
-      <c r="N45" s="17"/>
-      <c r="O45" s="17"/>
-      <c r="P45" s="17"/>
-      <c r="Q45" s="17"/>
-      <c r="R45" s="17"/>
-      <c r="S45" s="17"/>
-      <c r="T45" s="17"/>
-      <c r="U45" s="17"/>
-      <c r="V45" s="17"/>
-      <c r="W45" s="17"/>
-      <c r="X45" s="15">
-        <v>44</v>
-      </c>
-      <c r="Y45" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z45" s="15" t="s">
+      <c r="G45" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
+      <c r="N45" s="27"/>
+      <c r="O45" s="27"/>
+      <c r="P45" s="27"/>
+      <c r="Q45" s="27"/>
+      <c r="R45" s="27"/>
+      <c r="S45" s="27"/>
+      <c r="T45" s="27"/>
+      <c r="U45" s="27"/>
+      <c r="V45" s="27"/>
+      <c r="W45" s="27"/>
+      <c r="X45" s="28">
+        <v>47</v>
+      </c>
+      <c r="Y45" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z45" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="AA45" s="15" t="s">
+      <c r="AA45" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="AB45" s="17"/>
-      <c r="AC45" s="15">
-        <v>46</v>
-      </c>
-      <c r="AD45" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE45" s="15" t="s">
+      <c r="AB45" s="27"/>
+      <c r="AC45" s="28">
+        <v>55</v>
+      </c>
+      <c r="AD45" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE45" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="AF45" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG45" s="9"/>
-      <c r="AH45" s="9" t="s">
+      <c r="AF45" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG45" s="28"/>
+      <c r="AH45" s="28">
+        <v>57</v>
+      </c>
+      <c r="AI45" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="AJ45" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK45" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL45" s="28"/>
+      <c r="AM45" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="AI45" s="17"/>
-      <c r="AJ45" s="9"/>
-      <c r="AK45" s="9"/>
-      <c r="AL45" s="9"/>
-      <c r="AM45" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="AN45" s="17"/>
-      <c r="AO45" s="9"/>
-      <c r="AP45" s="9"/>
-      <c r="AQ45" s="9"/>
-      <c r="AR45" s="9"/>
-      <c r="AS45" s="9"/>
-      <c r="AT45" s="9"/>
-      <c r="AU45" s="9"/>
-      <c r="AV45" s="9"/>
-      <c r="AW45" s="9"/>
-      <c r="AX45" s="9"/>
-      <c r="AY45" s="9"/>
-      <c r="AZ45" s="9"/>
-      <c r="BA45" s="9"/>
-      <c r="BB45" s="9"/>
-      <c r="BC45" s="9"/>
+      <c r="AN45" s="27"/>
+      <c r="AO45" s="28"/>
+      <c r="AP45" s="28"/>
+      <c r="AQ45" s="28"/>
+      <c r="AR45" s="28"/>
+      <c r="AS45" s="28"/>
+      <c r="AT45" s="28"/>
+      <c r="AU45" s="28"/>
+      <c r="AV45" s="28"/>
+      <c r="AW45" s="28"/>
+      <c r="AX45" s="28"/>
+      <c r="AY45" s="28"/>
+      <c r="AZ45" s="28"/>
+      <c r="BA45" s="28"/>
+      <c r="BB45" s="28"/>
+      <c r="BC45" s="28"/>
     </row>
     <row r="46" spans="1:55" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
@@ -5374,10 +5378,10 @@
         <v>44</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="E46" s="18" t="s">
         <v>113</v>
@@ -5386,14 +5390,12 @@
         <v>21</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="I46" s="18" t="s">
-        <v>145</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="I46" s="18"/>
       <c r="J46" s="17"/>
       <c r="K46" s="17"/>
       <c r="L46" s="17"/>
@@ -5409,42 +5411,37 @@
       <c r="V46" s="17"/>
       <c r="W46" s="17"/>
       <c r="X46" s="15">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="Y46" s="18" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="Z46" s="15" t="s">
         <v>22</v>
       </c>
       <c r="AA46" s="15" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="AB46" s="17"/>
-      <c r="AC46" s="15">
-        <v>46</v>
-      </c>
-      <c r="AD46" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE46" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF46" s="33" t="s">
-        <v>39</v>
-      </c>
+      <c r="AC46" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AD46" s="17"/>
+      <c r="AE46" s="9"/>
+      <c r="AF46" s="9"/>
       <c r="AG46" s="9"/>
       <c r="AH46" s="9" t="s">
         <v>205</v>
       </c>
       <c r="AI46" s="17"/>
       <c r="AJ46" s="9"/>
-      <c r="AK46" s="9"/>
       <c r="AL46" s="9"/>
-      <c r="AM46" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="AN46" s="17"/>
+      <c r="AM46" s="15">
+        <v>46</v>
+      </c>
+      <c r="AN46" s="18" t="s">
+        <v>158</v>
+      </c>
       <c r="AO46" s="9"/>
       <c r="AP46" s="9"/>
       <c r="AQ46" s="9"/>
@@ -5462,17 +5459,17 @@
       <c r="BC46" s="9"/>
     </row>
     <row r="47" spans="1:55" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="23" t="s">
-        <v>126</v>
+      <c r="A47" s="22" t="s">
+        <v>111</v>
       </c>
       <c r="B47" s="20">
         <v>45</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="E47" s="18" t="s">
         <v>113</v>
@@ -5481,23 +5478,21 @@
         <v>21</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="H47" s="18" t="s">
-        <v>128</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="H47" s="17"/>
       <c r="I47" s="17"/>
-      <c r="J47" s="34" t="s">
-        <v>212</v>
+      <c r="J47" s="18" t="s">
+        <v>85</v>
       </c>
       <c r="K47" s="18" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="L47" s="18" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="M47" s="18" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="N47" s="17"/>
       <c r="O47" s="17"/>
@@ -5509,8 +5504,11 @@
       <c r="U47" s="17"/>
       <c r="V47" s="17"/>
       <c r="W47" s="17"/>
-      <c r="Y47" s="26" t="s">
-        <v>206</v>
+      <c r="X47" s="15">
+        <v>49</v>
+      </c>
+      <c r="Y47" s="18" t="s">
+        <v>164</v>
       </c>
       <c r="Z47" s="24" t="s">
         <v>22</v>
@@ -5518,34 +5516,38 @@
       <c r="AA47" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AB47" s="18" t="s">
-        <v>209</v>
-      </c>
+      <c r="AB47" s="17"/>
       <c r="AC47" s="15">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="AD47" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="AE47" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="AE47" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AF47" s="15" t="s">
+      <c r="AF47" s="24" t="s">
         <v>31</v>
       </c>
       <c r="AG47" s="9"/>
-      <c r="AH47" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="AI47" s="17"/>
-      <c r="AJ47" s="9"/>
-      <c r="AK47" s="9"/>
+      <c r="AH47" s="15">
+        <v>53</v>
+      </c>
+      <c r="AI47" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="AJ47" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK47" s="24" t="s">
+        <v>23</v>
+      </c>
       <c r="AL47" s="9"/>
       <c r="AM47" s="15">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="AN47" s="18" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="AO47" s="9"/>
       <c r="AP47" s="9"/>
@@ -5563,116 +5565,117 @@
       <c r="BB47" s="9"/>
       <c r="BC47" s="9"/>
     </row>
-    <row r="48" spans="1:55" s="32" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:55" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
         <v>111</v>
       </c>
       <c r="B48" s="20">
         <v>46</v>
       </c>
-      <c r="C48" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="D48" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="E48" s="30" t="s">
+      <c r="C48" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E48" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="F48" s="31" t="s">
+      <c r="F48" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G48" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="H48" s="30"/>
-      <c r="I48" s="30"/>
-      <c r="J48" s="30"/>
-      <c r="K48" s="30"/>
-      <c r="L48" s="30"/>
-      <c r="M48" s="30"/>
-      <c r="N48" s="30"/>
-      <c r="O48" s="30"/>
-      <c r="P48" s="30"/>
-      <c r="Q48" s="30"/>
-      <c r="R48" s="30"/>
-      <c r="S48" s="30"/>
-      <c r="T48" s="30"/>
-      <c r="U48" s="30"/>
-      <c r="V48" s="30"/>
-      <c r="W48" s="30"/>
-      <c r="X48" s="31">
-        <v>47</v>
-      </c>
-      <c r="Y48" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="Z48" s="31" t="s">
+      <c r="G48" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="L48" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M48" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="N48" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="O48" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="P48" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q48" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="R48" s="17"/>
+      <c r="S48" s="17"/>
+      <c r="T48" s="17"/>
+      <c r="U48" s="17"/>
+      <c r="V48" s="17"/>
+      <c r="W48" s="17"/>
+      <c r="X48" s="15">
+        <v>50</v>
+      </c>
+      <c r="Y48" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z48" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AA48" s="31" t="s">
+      <c r="AA48" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AB48" s="30"/>
-      <c r="AC48" s="31">
-        <v>55</v>
-      </c>
-      <c r="AD48" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="AE48" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF48" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG48" s="31"/>
-      <c r="AH48" s="31">
-        <v>57</v>
-      </c>
-      <c r="AI48" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="AJ48" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK48" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="AL48" s="31"/>
-      <c r="AM48" s="31" t="s">
+      <c r="AB48" s="17"/>
+      <c r="AC48" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="AN48" s="30"/>
-      <c r="AO48" s="31"/>
-      <c r="AP48" s="31"/>
-      <c r="AQ48" s="31"/>
-      <c r="AR48" s="31"/>
-      <c r="AS48" s="31"/>
-      <c r="AT48" s="31"/>
-      <c r="AU48" s="31"/>
-      <c r="AV48" s="31"/>
-      <c r="AW48" s="31"/>
-      <c r="AX48" s="31"/>
-      <c r="AY48" s="31"/>
-      <c r="AZ48" s="31"/>
-      <c r="BA48" s="31"/>
-      <c r="BB48" s="31"/>
-      <c r="BC48" s="31"/>
+      <c r="AD48" s="17"/>
+      <c r="AE48" s="9"/>
+      <c r="AF48" s="9"/>
+      <c r="AG48" s="9"/>
+      <c r="AH48" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AI48" s="17"/>
+      <c r="AJ48" s="9"/>
+      <c r="AK48" s="9"/>
+      <c r="AL48" s="9"/>
+      <c r="AM48" s="15">
+        <v>48</v>
+      </c>
+      <c r="AN48" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="AO48" s="9"/>
+      <c r="AP48" s="9"/>
+      <c r="AQ48" s="9"/>
+      <c r="AR48" s="9"/>
+      <c r="AS48" s="9"/>
+      <c r="AT48" s="9"/>
+      <c r="AU48" s="9"/>
+      <c r="AV48" s="9"/>
+      <c r="AW48" s="9"/>
+      <c r="AX48" s="9"/>
+      <c r="AY48" s="9"/>
+      <c r="AZ48" s="9"/>
+      <c r="BA48" s="9"/>
+      <c r="BB48" s="9"/>
+      <c r="BC48" s="9"/>
     </row>
     <row r="49" spans="1:55" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="22" t="s">
-        <v>111</v>
+      <c r="A49" s="23" t="s">
+        <v>126</v>
       </c>
       <c r="B49" s="20">
         <v>47</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="D49" s="18" t="s">
-        <v>154</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="D49" s="18"/>
       <c r="E49" s="18" t="s">
         <v>113</v>
       </c>
@@ -5680,16 +5683,24 @@
         <v>21</v>
       </c>
       <c r="G49" s="18" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="I49" s="18"/>
-      <c r="J49" s="17"/>
-      <c r="K49" s="17"/>
-      <c r="L49" s="17"/>
-      <c r="M49" s="17"/>
+        <v>128</v>
+      </c>
+      <c r="I49" s="17"/>
+      <c r="J49" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="K49" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="L49" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="M49" s="18" t="s">
+        <v>131</v>
+      </c>
       <c r="N49" s="17"/>
       <c r="O49" s="17"/>
       <c r="P49" s="17"/>
@@ -5700,37 +5711,43 @@
       <c r="U49" s="17"/>
       <c r="V49" s="17"/>
       <c r="W49" s="17"/>
-      <c r="X49" s="15">
-        <v>48</v>
-      </c>
-      <c r="Y49" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="Z49" s="15" t="s">
+      <c r="Y49" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z49" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AA49" s="15" t="s">
+      <c r="AA49" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB49" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC49" s="9">
+        <v>62</v>
+      </c>
+      <c r="AD49" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE49" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF49" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AB49" s="17"/>
-      <c r="AC49" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="AD49" s="17"/>
-      <c r="AE49" s="9"/>
-      <c r="AF49" s="9"/>
       <c r="AG49" s="9"/>
       <c r="AH49" s="9" t="s">
         <v>205</v>
       </c>
       <c r="AI49" s="17"/>
       <c r="AJ49" s="9"/>
+      <c r="AK49" s="9"/>
       <c r="AL49" s="9"/>
       <c r="AM49" s="15">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="AN49" s="18" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="AO49" s="9"/>
       <c r="AP49" s="9"/>
@@ -5756,11 +5773,9 @@
         <v>48</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>159</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="D50" s="17"/>
       <c r="E50" s="18" t="s">
         <v>113</v>
       </c>
@@ -5768,22 +5783,22 @@
         <v>21</v>
       </c>
       <c r="G50" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="H50" s="17"/>
+        <v>178</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>168</v>
+      </c>
       <c r="I50" s="17"/>
       <c r="J50" s="18" t="s">
         <v>85</v>
       </c>
       <c r="K50" s="18" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="L50" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="M50" s="18" t="s">
-        <v>163</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="M50" s="17"/>
       <c r="N50" s="17"/>
       <c r="O50" s="17"/>
       <c r="P50" s="17"/>
@@ -5795,49 +5810,37 @@
       <c r="V50" s="17"/>
       <c r="W50" s="17"/>
       <c r="X50" s="15">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="Y50" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="Z50" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z50" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AA50" s="24" t="s">
+      <c r="AA50" s="15" t="s">
         <v>38</v>
       </c>
       <c r="AB50" s="17"/>
-      <c r="AC50" s="15">
-        <v>51</v>
-      </c>
-      <c r="AD50" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="AE50" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF50" s="24" t="s">
-        <v>31</v>
-      </c>
+      <c r="AC50" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AD50" s="17"/>
+      <c r="AE50" s="9"/>
+      <c r="AF50" s="9"/>
       <c r="AG50" s="9"/>
-      <c r="AH50" s="15">
-        <v>53</v>
-      </c>
-      <c r="AI50" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="AJ50" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK50" s="24" t="s">
-        <v>23</v>
-      </c>
+      <c r="AH50" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AI50" s="17"/>
+      <c r="AJ50" s="9"/>
+      <c r="AK50" s="9"/>
       <c r="AL50" s="9"/>
       <c r="AM50" s="15">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AN50" s="18" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="AO50" s="9"/>
       <c r="AP50" s="9"/>
@@ -5856,15 +5859,16 @@
       <c r="BC50" s="9"/>
     </row>
     <row r="51" spans="1:55" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="22" t="s">
-        <v>111</v>
+      <c r="A51" s="23" t="s">
+        <v>126</v>
       </c>
       <c r="B51" s="20">
         <v>49</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>164</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="D51" s="18"/>
       <c r="E51" s="18" t="s">
         <v>113</v>
       </c>
@@ -5872,59 +5876,58 @@
         <v>21</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>167</v>
+        <v>127</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>168</v>
+        <v>128</v>
       </c>
       <c r="I51" s="17"/>
-      <c r="J51" s="17"/>
+      <c r="J51" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="K51" s="18" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
       <c r="L51" s="18" t="s">
-        <v>170</v>
+        <v>130</v>
       </c>
       <c r="M51" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="N51" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="O51" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="P51" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q51" s="18" t="s">
-        <v>175</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="N51" s="17"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17"/>
+      <c r="Q51" s="17"/>
       <c r="R51" s="17"/>
       <c r="S51" s="17"/>
       <c r="T51" s="17"/>
       <c r="U51" s="17"/>
       <c r="V51" s="17"/>
       <c r="W51" s="17"/>
-      <c r="X51" s="15">
-        <v>50</v>
-      </c>
-      <c r="Y51" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="Z51" s="15" t="s">
+      <c r="Y51" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z51" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AA51" s="15" t="s">
+      <c r="AA51" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AB51" s="17"/>
-      <c r="AC51" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="AD51" s="17"/>
-      <c r="AE51" s="9"/>
-      <c r="AF51" s="9"/>
+      <c r="AB51" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC51" s="15">
+        <v>63</v>
+      </c>
+      <c r="AD51" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE51" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF51" s="15" t="s">
+        <v>31</v>
+      </c>
       <c r="AG51" s="9"/>
       <c r="AH51" s="9" t="s">
         <v>205</v>
@@ -5934,10 +5937,10 @@
       <c r="AK51" s="9"/>
       <c r="AL51" s="9"/>
       <c r="AM51" s="15">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="AN51" s="18" t="s">
-        <v>177</v>
+        <v>133</v>
       </c>
       <c r="AO51" s="9"/>
       <c r="AP51" s="9"/>
@@ -5956,16 +5959,16 @@
       <c r="BC51" s="9"/>
     </row>
     <row r="52" spans="1:55" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="23" t="s">
-        <v>126</v>
+      <c r="A52" s="22" t="s">
+        <v>111</v>
       </c>
       <c r="B52" s="20">
         <v>50</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="D52" s="18"/>
+        <v>166</v>
+      </c>
+      <c r="D52" s="17"/>
       <c r="E52" s="18" t="s">
         <v>113</v>
       </c>
@@ -5973,24 +5976,14 @@
         <v>21</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="H52" s="18" t="s">
-        <v>128</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="H52" s="17"/>
       <c r="I52" s="17"/>
-      <c r="J52" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="K52" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="L52" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="M52" s="18" t="s">
-        <v>131</v>
-      </c>
+      <c r="J52" s="17"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="M52" s="17"/>
       <c r="N52" s="17"/>
       <c r="O52" s="17"/>
       <c r="P52" s="17"/>
@@ -6001,30 +5994,25 @@
       <c r="U52" s="17"/>
       <c r="V52" s="17"/>
       <c r="W52" s="17"/>
-      <c r="Y52" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="Z52" s="24" t="s">
+      <c r="X52" s="15">
+        <v>54</v>
+      </c>
+      <c r="Y52" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z52" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AA52" s="24" t="s">
+      <c r="AA52" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AB52" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="AC52" s="9">
-        <v>62</v>
-      </c>
-      <c r="AD52" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="AE52" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF52" s="15" t="s">
-        <v>31</v>
-      </c>
+      <c r="AB52" s="17"/>
+      <c r="AC52" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AD52" s="17"/>
+      <c r="AE52" s="9"/>
+      <c r="AF52" s="9"/>
       <c r="AG52" s="9"/>
       <c r="AH52" s="9" t="s">
         <v>205</v>
@@ -6034,10 +6022,10 @@
       <c r="AK52" s="9"/>
       <c r="AL52" s="9"/>
       <c r="AM52" s="15">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="AN52" s="18" t="s">
-        <v>133</v>
+        <v>177</v>
       </c>
       <c r="AO52" s="9"/>
       <c r="AP52" s="9"/>
@@ -6056,16 +6044,16 @@
       <c r="BC52" s="9"/>
     </row>
     <row r="53" spans="1:55" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="22" t="s">
-        <v>111</v>
+      <c r="A53" s="23" t="s">
+        <v>126</v>
       </c>
       <c r="B53" s="20">
         <v>51</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D53" s="17"/>
+        <v>166</v>
+      </c>
+      <c r="D53" s="18"/>
       <c r="E53" s="18" t="s">
         <v>113</v>
       </c>
@@ -6073,22 +6061,24 @@
         <v>21</v>
       </c>
       <c r="G53" s="18" t="s">
-        <v>178</v>
+        <v>127</v>
       </c>
       <c r="H53" s="18" t="s">
-        <v>168</v>
+        <v>128</v>
       </c>
       <c r="I53" s="17"/>
-      <c r="J53" s="18" t="s">
-        <v>85</v>
+      <c r="J53" s="31" t="s">
+        <v>212</v>
       </c>
       <c r="K53" s="18" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="L53" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="M53" s="17"/>
+        <v>130</v>
+      </c>
+      <c r="M53" s="18" t="s">
+        <v>131</v>
+      </c>
       <c r="N53" s="17"/>
       <c r="O53" s="17"/>
       <c r="P53" s="17"/>
@@ -6099,25 +6089,30 @@
       <c r="U53" s="17"/>
       <c r="V53" s="17"/>
       <c r="W53" s="17"/>
-      <c r="X53" s="15">
-        <v>52</v>
-      </c>
-      <c r="Y53" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="Z53" s="15" t="s">
+      <c r="Y53" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z53" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AA53" s="15" t="s">
+      <c r="AA53" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AB53" s="17"/>
-      <c r="AC53" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="AD53" s="17"/>
-      <c r="AE53" s="9"/>
-      <c r="AF53" s="9"/>
+      <c r="AB53" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC53" s="15">
+        <v>64</v>
+      </c>
+      <c r="AD53" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE53" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF53" s="15" t="s">
+        <v>31</v>
+      </c>
       <c r="AG53" s="9"/>
       <c r="AH53" s="9" t="s">
         <v>205</v>
@@ -6127,10 +6122,10 @@
       <c r="AK53" s="9"/>
       <c r="AL53" s="9"/>
       <c r="AM53" s="15">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="AN53" s="18" t="s">
-        <v>177</v>
+        <v>133</v>
       </c>
       <c r="AO53" s="9"/>
       <c r="AP53" s="9"/>
@@ -6149,16 +6144,18 @@
       <c r="BC53" s="9"/>
     </row>
     <row r="54" spans="1:55" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="23" t="s">
-        <v>126</v>
+      <c r="A54" s="22" t="s">
+        <v>111</v>
       </c>
       <c r="B54" s="20">
         <v>52</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D54" s="18"/>
+        <v>184</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>185</v>
+      </c>
       <c r="E54" s="18" t="s">
         <v>113</v>
       </c>
@@ -6166,24 +6163,18 @@
         <v>21</v>
       </c>
       <c r="G54" s="18" t="s">
-        <v>127</v>
+        <v>186</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="I54" s="17"/>
-      <c r="J54" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="K54" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="L54" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="M54" s="18" t="s">
-        <v>131</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="I54" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="J54" s="17"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
       <c r="N54" s="17"/>
       <c r="O54" s="17"/>
       <c r="P54" s="17"/>
@@ -6194,30 +6185,25 @@
       <c r="U54" s="17"/>
       <c r="V54" s="17"/>
       <c r="W54" s="17"/>
-      <c r="Y54" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="Z54" s="24" t="s">
+      <c r="X54" s="15">
+        <v>56</v>
+      </c>
+      <c r="Y54" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z54" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AA54" s="24" t="s">
+      <c r="AA54" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AB54" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="AC54" s="15">
-        <v>63</v>
-      </c>
-      <c r="AD54" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="AE54" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF54" s="15" t="s">
-        <v>31</v>
-      </c>
+      <c r="AB54" s="17"/>
+      <c r="AC54" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AD54" s="17"/>
+      <c r="AE54" s="9"/>
+      <c r="AF54" s="9"/>
       <c r="AG54" s="9"/>
       <c r="AH54" s="9" t="s">
         <v>205</v>
@@ -6227,10 +6213,10 @@
       <c r="AK54" s="9"/>
       <c r="AL54" s="9"/>
       <c r="AM54" s="15">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="AN54" s="18" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="AO54" s="9"/>
       <c r="AP54" s="9"/>
@@ -6249,16 +6235,18 @@
       <c r="BC54" s="9"/>
     </row>
     <row r="55" spans="1:55" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="22" t="s">
-        <v>111</v>
+      <c r="A55" s="23" t="s">
+        <v>126</v>
       </c>
       <c r="B55" s="20">
         <v>53</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="D55" s="17"/>
+        <v>184</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>185</v>
+      </c>
       <c r="E55" s="18" t="s">
         <v>113</v>
       </c>
@@ -6266,14 +6254,24 @@
         <v>21</v>
       </c>
       <c r="G55" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="H55" s="17"/>
+        <v>127</v>
+      </c>
+      <c r="H55" s="18" t="s">
+        <v>128</v>
+      </c>
       <c r="I55" s="17"/>
-      <c r="J55" s="17"/>
-      <c r="K55" s="17"/>
-      <c r="L55" s="17"/>
-      <c r="M55" s="17"/>
+      <c r="J55" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="K55" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="L55" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="M55" s="18" t="s">
+        <v>131</v>
+      </c>
       <c r="N55" s="17"/>
       <c r="O55" s="17"/>
       <c r="P55" s="17"/>
@@ -6284,25 +6282,30 @@
       <c r="U55" s="17"/>
       <c r="V55" s="17"/>
       <c r="W55" s="17"/>
-      <c r="X55" s="15">
-        <v>54</v>
-      </c>
-      <c r="Y55" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="Z55" s="15" t="s">
+      <c r="Y55" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z55" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AA55" s="15" t="s">
+      <c r="AA55" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AB55" s="17"/>
-      <c r="AC55" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="AD55" s="17"/>
-      <c r="AE55" s="9"/>
-      <c r="AF55" s="9"/>
+      <c r="AB55" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="AC55" s="15">
+        <v>65</v>
+      </c>
+      <c r="AD55" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE55" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF55" s="15" t="s">
+        <v>31</v>
+      </c>
       <c r="AG55" s="9"/>
       <c r="AH55" s="9" t="s">
         <v>205</v>
@@ -6312,10 +6315,10 @@
       <c r="AK55" s="9"/>
       <c r="AL55" s="9"/>
       <c r="AM55" s="15">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="AN55" s="18" t="s">
-        <v>177</v>
+        <v>133</v>
       </c>
       <c r="AO55" s="9"/>
       <c r="AP55" s="9"/>
@@ -6334,16 +6337,18 @@
       <c r="BC55" s="9"/>
     </row>
     <row r="56" spans="1:55" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="23" t="s">
-        <v>126</v>
+      <c r="A56" s="22" t="s">
+        <v>111</v>
       </c>
       <c r="B56" s="20">
         <v>54</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="D56" s="18"/>
+        <v>190</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>191</v>
+      </c>
       <c r="E56" s="18" t="s">
         <v>113</v>
       </c>
@@ -6351,24 +6356,18 @@
         <v>21</v>
       </c>
       <c r="G56" s="18" t="s">
-        <v>127</v>
+        <v>192</v>
       </c>
       <c r="H56" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="I56" s="17"/>
-      <c r="J56" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="K56" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="L56" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="M56" s="18" t="s">
-        <v>131</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="I56" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
       <c r="N56" s="17"/>
       <c r="O56" s="17"/>
       <c r="P56" s="17"/>
@@ -6379,30 +6378,25 @@
       <c r="U56" s="17"/>
       <c r="V56" s="17"/>
       <c r="W56" s="17"/>
-      <c r="Y56" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="Z56" s="24" t="s">
+      <c r="X56" s="15">
+        <v>58</v>
+      </c>
+      <c r="Y56" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z56" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AA56" s="24" t="s">
+      <c r="AA56" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AB56" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="AC56" s="15">
-        <v>64</v>
-      </c>
-      <c r="AD56" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="AE56" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF56" s="15" t="s">
-        <v>31</v>
-      </c>
+      <c r="AB56" s="17"/>
+      <c r="AC56" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AD56" s="17"/>
+      <c r="AE56" s="9"/>
+      <c r="AF56" s="9"/>
       <c r="AG56" s="9"/>
       <c r="AH56" s="9" t="s">
         <v>205</v>
@@ -6412,10 +6406,10 @@
       <c r="AK56" s="9"/>
       <c r="AL56" s="9"/>
       <c r="AM56" s="15">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="AN56" s="18" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="AO56" s="9"/>
       <c r="AP56" s="9"/>
@@ -6434,17 +6428,17 @@
       <c r="BC56" s="9"/>
     </row>
     <row r="57" spans="1:55" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="22" t="s">
-        <v>111</v>
+      <c r="A57" s="23" t="s">
+        <v>126</v>
       </c>
       <c r="B57" s="20">
         <v>55</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="E57" s="18" t="s">
         <v>113</v>
@@ -6453,18 +6447,24 @@
         <v>21</v>
       </c>
       <c r="G57" s="18" t="s">
-        <v>186</v>
+        <v>127</v>
       </c>
       <c r="H57" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="I57" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="J57" s="17"/>
-      <c r="K57" s="17"/>
-      <c r="L57" s="17"/>
-      <c r="M57" s="17"/>
+        <v>128</v>
+      </c>
+      <c r="I57" s="17"/>
+      <c r="J57" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="K57" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="L57" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="M57" s="18" t="s">
+        <v>131</v>
+      </c>
       <c r="N57" s="17"/>
       <c r="O57" s="17"/>
       <c r="P57" s="17"/>
@@ -6475,25 +6475,30 @@
       <c r="U57" s="17"/>
       <c r="V57" s="17"/>
       <c r="W57" s="17"/>
-      <c r="X57" s="15">
-        <v>56</v>
-      </c>
-      <c r="Y57" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="Z57" s="15" t="s">
+      <c r="Y57" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z57" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AA57" s="15" t="s">
+      <c r="AA57" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AB57" s="17"/>
-      <c r="AC57" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="AD57" s="17"/>
-      <c r="AE57" s="9"/>
-      <c r="AF57" s="9"/>
+      <c r="AB57" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="AC57" s="15">
+        <v>66</v>
+      </c>
+      <c r="AD57" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE57" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF57" s="15" t="s">
+        <v>31</v>
+      </c>
       <c r="AG57" s="9"/>
       <c r="AH57" s="9" t="s">
         <v>205</v>
@@ -6503,10 +6508,10 @@
       <c r="AK57" s="9"/>
       <c r="AL57" s="9"/>
       <c r="AM57" s="15">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="AN57" s="18" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="AO57" s="9"/>
       <c r="AP57" s="9"/>
@@ -6525,17 +6530,17 @@
       <c r="BC57" s="9"/>
     </row>
     <row r="58" spans="1:55" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="23" t="s">
-        <v>126</v>
+      <c r="A58" s="22" t="s">
+        <v>111</v>
       </c>
       <c r="B58" s="20">
         <v>56</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>184</v>
+        <v>118</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>185</v>
+        <v>119</v>
       </c>
       <c r="E58" s="18" t="s">
         <v>113</v>
@@ -6544,24 +6549,18 @@
         <v>21</v>
       </c>
       <c r="G58" s="18" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H58" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="I58" s="17"/>
-      <c r="J58" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="K58" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="L58" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="M58" s="18" t="s">
-        <v>131</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="I58" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="J58" s="17"/>
+      <c r="K58" s="17"/>
+      <c r="L58" s="17"/>
+      <c r="M58" s="17"/>
       <c r="N58" s="17"/>
       <c r="O58" s="17"/>
       <c r="P58" s="17"/>
@@ -6572,29 +6571,30 @@
       <c r="U58" s="17"/>
       <c r="V58" s="17"/>
       <c r="W58" s="17"/>
-      <c r="Y58" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="Z58" s="24" t="s">
+      <c r="X58" s="15">
+        <v>38</v>
+      </c>
+      <c r="Y58" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z58" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AA58" s="24" t="s">
+      <c r="AA58" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AB58" s="18" t="s">
-        <v>211</v>
-      </c>
+      <c r="AB58" s="17"/>
       <c r="AC58" s="15">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="AD58" s="18" t="s">
-        <v>132</v>
+        <v>37</v>
       </c>
       <c r="AE58" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AF58" s="15" t="s">
-        <v>31</v>
+      <c r="AF58" s="30" t="s">
+        <v>39</v>
       </c>
       <c r="AG58" s="9"/>
       <c r="AH58" s="9" t="s">
@@ -6604,12 +6604,10 @@
       <c r="AJ58" s="9"/>
       <c r="AK58" s="9"/>
       <c r="AL58" s="9"/>
-      <c r="AM58" s="15">
-        <v>36</v>
-      </c>
-      <c r="AN58" s="18" t="s">
-        <v>133</v>
-      </c>
+      <c r="AM58" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="AN58" s="18"/>
       <c r="AO58" s="9"/>
       <c r="AP58" s="9"/>
       <c r="AQ58" s="9"/>
@@ -6634,10 +6632,10 @@
         <v>57</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>190</v>
+        <v>118</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>191</v>
+        <v>119</v>
       </c>
       <c r="E59" s="18" t="s">
         <v>113</v>
@@ -6646,14 +6644,12 @@
         <v>21</v>
       </c>
       <c r="G59" s="18" t="s">
-        <v>192</v>
+        <v>123</v>
       </c>
       <c r="H59" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="I59" s="18" t="s">
-        <v>188</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="I59" s="18"/>
       <c r="J59" s="17"/>
       <c r="K59" s="17"/>
       <c r="L59" s="17"/>
@@ -6669,10 +6665,10 @@
       <c r="V59" s="17"/>
       <c r="W59" s="17"/>
       <c r="X59" s="15">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="Y59" s="18" t="s">
-        <v>194</v>
+        <v>125</v>
       </c>
       <c r="Z59" s="15" t="s">
         <v>22</v>
@@ -6681,12 +6677,18 @@
         <v>38</v>
       </c>
       <c r="AB59" s="17"/>
-      <c r="AC59" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="AD59" s="17"/>
-      <c r="AE59" s="9"/>
-      <c r="AF59" s="9"/>
+      <c r="AC59" s="15">
+        <v>40</v>
+      </c>
+      <c r="AD59" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE59" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF59" s="30" t="s">
+        <v>39</v>
+      </c>
       <c r="AG59" s="9"/>
       <c r="AH59" s="9" t="s">
         <v>205</v>
@@ -6695,12 +6697,10 @@
       <c r="AJ59" s="9"/>
       <c r="AK59" s="9"/>
       <c r="AL59" s="9"/>
-      <c r="AM59" s="15">
-        <v>46</v>
-      </c>
-      <c r="AN59" s="18" t="s">
-        <v>158</v>
-      </c>
+      <c r="AM59" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="AN59" s="18"/>
       <c r="AO59" s="9"/>
       <c r="AP59" s="9"/>
       <c r="AQ59" s="9"/>
@@ -6725,10 +6725,10 @@
         <v>58</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>190</v>
+        <v>118</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>191</v>
+        <v>119</v>
       </c>
       <c r="E60" s="18" t="s">
         <v>113</v>
@@ -6743,7 +6743,7 @@
         <v>128</v>
       </c>
       <c r="I60" s="17"/>
-      <c r="J60" s="34" t="s">
+      <c r="J60" s="31" t="s">
         <v>212</v>
       </c>
       <c r="K60" s="18" t="s">
@@ -6775,10 +6775,10 @@
         <v>38</v>
       </c>
       <c r="AB60" s="18" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="AC60" s="15">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="AD60" s="18" t="s">
         <v>132</v>

</xml_diff>

<commit_message>
corrected links in lrt to match new scheam in form support
</commit_message>
<xml_diff>
--- a/make_lrt_json/LAT-content_Mod1_2.xlsx
+++ b/make_lrt_json/LAT-content_Mod1_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tamika.dual\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiadhgrandt-nesher/Workbench/aaa/make_lrt_json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204BC809-28E8-4E4A-AF72-6DF987B70E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157B4526-7034-4B4A-87F3-05B87D9088A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="-14980" windowWidth="67200" windowHeight="37300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Content by Screen" sheetId="1" r:id="rId1"/>
@@ -836,22 +836,22 @@
     <t>https://offices.sc.egov.usda.gov/locator/app?state=us&amp;agency=fsa</t>
   </si>
   <si>
-    <t>/walkthrough.html?youth</t>
+    <t>/walkthrough.html?loan_type=youth</t>
   </si>
   <si>
-    <t>/walkthrough.html?emergency</t>
+    <t>/walkthrough.html?loan_type=emergency</t>
   </si>
   <si>
-    <t>/walkthrough.html?microloan</t>
+    <t>/walkthrough.html?loan_type=microloan</t>
   </si>
   <si>
-    <t>/walkthrough.html?ownership</t>
+    <t>/walkthrough.html?loan_type=ownership</t>
   </si>
   <si>
-    <t>/walkthrough.html?term</t>
+    <t>/walkthrough.html?loan_type=term</t>
   </si>
   <si>
-    <t>/walkthrough.html?annual</t>
+    <t>/walkthrough.html?loan_type=annual</t>
   </si>
 </sst>
 </file>
@@ -1581,50 +1581,50 @@
   </sheetPr>
   <dimension ref="A1:BC1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="X60" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="6" ySplit="2" topLeftCell="X40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y73" sqref="Y73"/>
+      <selection pane="bottomRight" activeCell="AB61" sqref="AB61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" customWidth="1"/>
-    <col min="2" max="2" width="3.26953125" customWidth="1"/>
-    <col min="3" max="3" width="21.453125" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="3.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" customWidth="1"/>
-    <col min="7" max="7" width="30.26953125" customWidth="1"/>
-    <col min="8" max="8" width="29.7265625" customWidth="1"/>
-    <col min="9" max="9" width="29.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" customWidth="1"/>
+    <col min="9" max="9" width="29.5" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="12" max="12" width="16.08984375" customWidth="1"/>
-    <col min="14" max="14" width="13.453125" customWidth="1"/>
-    <col min="15" max="15" width="13.08984375" customWidth="1"/>
+    <col min="12" max="12" width="16.1640625" customWidth="1"/>
+    <col min="14" max="14" width="13.5" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="20" max="20" width="14.08984375" customWidth="1"/>
-    <col min="21" max="21" width="13.81640625" customWidth="1"/>
-    <col min="22" max="22" width="22.08984375" customWidth="1"/>
-    <col min="23" max="23" width="11.7265625" customWidth="1"/>
-    <col min="24" max="24" width="10.453125" customWidth="1"/>
-    <col min="25" max="25" width="13.453125" customWidth="1"/>
-    <col min="26" max="26" width="7.08984375" customWidth="1"/>
-    <col min="27" max="27" width="10.08984375" customWidth="1"/>
-    <col min="28" max="28" width="25.26953125" customWidth="1"/>
-    <col min="29" max="29" width="11.7265625" customWidth="1"/>
-    <col min="30" max="30" width="10.453125" customWidth="1"/>
-    <col min="31" max="31" width="5.453125" customWidth="1"/>
+    <col min="20" max="20" width="14.1640625" customWidth="1"/>
+    <col min="21" max="21" width="13.83203125" customWidth="1"/>
+    <col min="22" max="22" width="22.1640625" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" customWidth="1"/>
+    <col min="24" max="24" width="10.5" customWidth="1"/>
+    <col min="25" max="25" width="13.5" customWidth="1"/>
+    <col min="26" max="26" width="7.1640625" customWidth="1"/>
+    <col min="27" max="27" width="10.1640625" customWidth="1"/>
+    <col min="28" max="28" width="25.33203125" customWidth="1"/>
+    <col min="29" max="29" width="11.6640625" customWidth="1"/>
+    <col min="30" max="30" width="10.5" customWidth="1"/>
+    <col min="31" max="31" width="5.5" customWidth="1"/>
     <col min="32" max="32" width="10" customWidth="1"/>
-    <col min="33" max="33" width="11.81640625" customWidth="1"/>
+    <col min="33" max="33" width="11.83203125" customWidth="1"/>
     <col min="34" max="34" width="12" customWidth="1"/>
     <col min="35" max="35" width="11" customWidth="1"/>
-    <col min="36" max="36" width="5.453125" customWidth="1"/>
+    <col min="36" max="36" width="5.5" customWidth="1"/>
     <col min="37" max="37" width="10" customWidth="1"/>
-    <col min="38" max="38" width="17.453125" customWidth="1"/>
+    <col min="38" max="38" width="17.5" customWidth="1"/>
     <col min="39" max="39" width="14" customWidth="1"/>
-    <col min="40" max="40" width="11.7265625" customWidth="1"/>
+    <col min="40" max="40" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:55">

</xml_diff>